<commit_message>
some unknown change in the excel file that probably doesn't matter
</commit_message>
<xml_diff>
--- a/Task 1 - article generation/Moroccan_politicians.xlsx
+++ b/Task 1 - article generation/Moroccan_politicians.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$F$1:$F$17</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -776,6 +779,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -784,10 +791,10 @@
   <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.71"/>
@@ -1787,6 +1794,27 @@
       </c>
       <c r="W17" s="2" t="s">
         <v>207</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="e">
+        <f aca="false">SUM(C20:C23)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="1048131" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2236,6 +2264,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <autoFilter ref="F1:F17"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://www.wikidata.org/entity/Q176490"/>
     <hyperlink ref="U2" r:id="rId2" display="https://en.wikipedia.org/wiki/Ahmed_Bahnini"/>
@@ -2308,5 +2337,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId64"/>
 </worksheet>
 </file>
</xml_diff>